<commit_message>
Market Share Excel Export
</commit_message>
<xml_diff>
--- a/Merck Sereno Dashboard/Dashboard/Content/ExportTemplate/MSLineChart.xlsx
+++ b/Merck Sereno Dashboard/Dashboard/Content/ExportTemplate/MSLineChart.xlsx
@@ -15,10 +15,33 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -56,9 +79,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -108,8 +134,8 @@
           <c:yMode val="edge"/>
           <c:x val="5.0623120491736791E-2"/>
           <c:y val="6.6470669494486559E-2"/>
-          <c:w val="0.82367936243671447"/>
-          <c:h val="0.8507567668592505"/>
+          <c:w val="0.76706468883763879"/>
+          <c:h val="0.75292646295814047"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -120,7 +146,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$31</c:f>
+              <c:f>Sheet1!$C$30</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
               </c:strCache>
@@ -131,19 +157,19 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$30:$AV$30</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="46"/>
+              <c:f>Sheet1!$D$29:$AV$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="45"/>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$31:$AV$31</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="46"/>
+              <c:f>Sheet1!$D$30:$AV$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="45"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -154,7 +180,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$32</c:f>
+              <c:f>Sheet1!$C$31</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
               </c:strCache>
@@ -172,19 +198,19 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$30:$AV$30</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="46"/>
+              <c:f>Sheet1!$D$29:$AV$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="45"/>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$32:$AV$32</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="46"/>
+              <c:f>Sheet1!$D$31:$AV$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="45"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -195,89 +221,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$33</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="12700">
-              <a:solidFill>
-                <a:srgbClr val="FFFF00"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$C$30:$AV$30</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="46"/>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$C$33:$AV$33</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="46"/>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$B$34</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="12700">
-              <a:solidFill>
-                <a:srgbClr val="00FFFF"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$C$30:$AV$30</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="46"/>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$C$34:$AV$34</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="46"/>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="4"/>
-          <c:order val="4"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$B$35</c:f>
+              <c:f>Sheet1!$C$32</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
               </c:strCache>
@@ -288,30 +232,30 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$30:$AV$30</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="46"/>
+              <c:f>Sheet1!$D$29:$AV$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="45"/>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$35:$AV$35</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="46"/>
+              <c:f>Sheet1!$D$32:$AV$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="45"/>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
         <c:ser>
-          <c:idx val="5"/>
-          <c:order val="5"/>
+          <c:idx val="3"/>
+          <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$36</c:f>
+              <c:f>Sheet1!$C$33</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
               </c:strCache>
@@ -322,30 +266,30 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$30:$AV$30</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="46"/>
+              <c:f>Sheet1!$D$29:$AV$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="45"/>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$36:$AV$36</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="46"/>
+              <c:f>Sheet1!$D$33:$AV$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="45"/>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
         <c:ser>
-          <c:idx val="6"/>
-          <c:order val="6"/>
+          <c:idx val="4"/>
+          <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$37</c:f>
+              <c:f>Sheet1!$C$34</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
               </c:strCache>
@@ -356,30 +300,30 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$30:$AV$30</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="46"/>
+              <c:f>Sheet1!$D$29:$AV$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="45"/>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$37:$AV$37</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="46"/>
+              <c:f>Sheet1!$D$34:$AV$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="45"/>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
         <c:ser>
-          <c:idx val="7"/>
-          <c:order val="7"/>
+          <c:idx val="5"/>
+          <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$38</c:f>
+              <c:f>Sheet1!$C$35</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
               </c:strCache>
@@ -390,30 +334,30 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$30:$AV$30</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="46"/>
+              <c:f>Sheet1!$D$29:$AV$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="45"/>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$38:$AV$38</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="46"/>
+              <c:f>Sheet1!$D$35:$AV$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="45"/>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
         <c:ser>
-          <c:idx val="8"/>
-          <c:order val="8"/>
+          <c:idx val="6"/>
+          <c:order val="6"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$39</c:f>
+              <c:f>Sheet1!$C$36</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
               </c:strCache>
@@ -424,30 +368,30 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$30:$AV$30</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="46"/>
+              <c:f>Sheet1!$D$29:$AV$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="45"/>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$39:$AV$39</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="46"/>
+              <c:f>Sheet1!$D$36:$AV$36</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="45"/>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
         <c:ser>
-          <c:idx val="9"/>
-          <c:order val="9"/>
+          <c:idx val="7"/>
+          <c:order val="7"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$40</c:f>
+              <c:f>Sheet1!$C$37</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
               </c:strCache>
@@ -458,30 +402,30 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$30:$AV$30</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="46"/>
+              <c:f>Sheet1!$D$29:$AV$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="45"/>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$40:$AV$40</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="46"/>
+              <c:f>Sheet1!$D$37:$AV$37</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="45"/>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
         <c:ser>
-          <c:idx val="10"/>
-          <c:order val="10"/>
+          <c:idx val="8"/>
+          <c:order val="8"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$41</c:f>
+              <c:f>Sheet1!$C$38</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
               </c:strCache>
@@ -492,30 +436,30 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$30:$AV$30</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="46"/>
+              <c:f>Sheet1!$D$29:$AV$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="45"/>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$41:$AV$41</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="46"/>
+              <c:f>Sheet1!$D$38:$AV$38</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="45"/>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
         <c:ser>
-          <c:idx val="11"/>
-          <c:order val="11"/>
+          <c:idx val="9"/>
+          <c:order val="9"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$42</c:f>
+              <c:f>Sheet1!$C$39</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
               </c:strCache>
@@ -526,30 +470,30 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$30:$AV$30</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="46"/>
+              <c:f>Sheet1!$D$29:$AV$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="45"/>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$42:$AV$42</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="46"/>
+              <c:f>Sheet1!$D$39:$AV$39</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="45"/>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
         <c:ser>
-          <c:idx val="12"/>
-          <c:order val="12"/>
+          <c:idx val="10"/>
+          <c:order val="10"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$43</c:f>
+              <c:f>Sheet1!$C$40</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
               </c:strCache>
@@ -560,87 +504,19 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$30:$AV$30</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="46"/>
+              <c:f>Sheet1!$D$29:$AV$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="45"/>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$43:$AV$43</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="46"/>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="13"/>
-          <c:order val="13"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$B$44</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$C$30:$AV$30</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="46"/>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$C$44:$AV$44</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="46"/>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="14"/>
-          <c:order val="14"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$B$45</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$C$30:$AV$30</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="46"/>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$C$45:$AV$45</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="46"/>
+              <c:f>Sheet1!$D$40:$AV$40</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="45"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -656,11 +532,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="679932416"/>
-        <c:axId val="695635328"/>
+        <c:axId val="543894528"/>
+        <c:axId val="109760448"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="679932416"/>
+        <c:axId val="543894528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -670,7 +546,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="695635328"/>
+        <c:crossAx val="109760448"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -678,7 +554,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="695635328"/>
+        <c:axId val="109760448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -688,7 +564,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="679932416"/>
+        <c:crossAx val="543894528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -699,10 +575,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.88132680122090457"/>
-          <c:y val="8.3496740672916198E-3"/>
-          <c:w val="0.11867319877909542"/>
-          <c:h val="0.97591712570993505"/>
+          <c:x val="0.86515118019259729"/>
+          <c:y val="2.4128844880814414E-2"/>
+          <c:w val="0.12824956672443674"/>
+          <c:h val="0.90939917183359542"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -742,7 +618,7 @@
       <xdr:col>19</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>114299</xdr:rowOff>
+      <xdr:rowOff>28574</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -773,14 +649,14 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
       <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>23812</xdr:rowOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1091,84 +967,66 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:S6"/>
+  <dimension ref="A3:S29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.140625" customWidth="1"/>
+    <col min="1" max="1" width="3.140625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
-      <c r="O4" s="2"/>
-      <c r="P4" s="2"/>
-      <c r="Q4" s="2"/>
-      <c r="R4" s="2"/>
+    <row r="3" spans="1:19" ht="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:19" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="5"/>
+      <c r="O4" s="5"/>
+      <c r="P4" s="5"/>
+      <c r="Q4" s="5"/>
+      <c r="R4" s="5"/>
       <c r="S4" s="1"/>
     </row>
-    <row r="5" spans="1:19" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
-      <c r="M5" s="2"/>
-      <c r="N5" s="2"/>
-      <c r="O5" s="2"/>
-      <c r="P5" s="2"/>
-      <c r="Q5" s="2"/>
-      <c r="R5" s="2"/>
-      <c r="S5" s="2"/>
+    <row r="5" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="6"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="6"/>
+      <c r="O5" s="6"/>
+      <c r="P5" s="6"/>
+      <c r="Q5" s="6"/>
+      <c r="R5" s="6"/>
+      <c r="S5" s="6"/>
     </row>
-    <row r="6" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
-      <c r="M6" s="3"/>
-      <c r="N6" s="3"/>
-      <c r="O6" s="3"/>
-      <c r="P6" s="3"/>
-      <c r="Q6" s="3"/>
-      <c r="R6" s="3"/>
-      <c r="S6" s="3"/>
+    <row r="29" spans="1:1" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="2">
     <mergeCell ref="A4:R4"/>
-    <mergeCell ref="A6:S6"/>
     <mergeCell ref="A5:S5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>